<commit_message>
upgrade and fix bug
增加了使用分布式锁对接口的幂等性检查、redisson实现接口限流、对接口类增加了totalNum及leftNum字段，并对修改接口调用次数的方法用@Transactional注解保证修改行锁的添加，保证数据一致性
</commit_message>
<xml_diff>
--- a/myapi-backend/src/main/resources/temp.xlsx
+++ b/myapi-backend/src/main/resources/temp.xlsx
@@ -27,42 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>月份</t>
   </si>
   <si>
     <t>访问量</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>号</t>
-    </r>
-  </si>
-  <si>
-    <t>2号</t>
-  </si>
-  <si>
-    <t>3号</t>
-  </si>
-  <si>
-    <t>4号</t>
-  </si>
-  <si>
-    <t>5号</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +999,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="22.8" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -1043,43 +1013,43 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>